<commit_message>
mise a jour de l'estimation
</commit_message>
<xml_diff>
--- a/Estimation des charges Horaires.xlsx
+++ b/Estimation des charges Horaires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanl\Desktop\3eme_cours_M2204\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeanl\Documents\DUT\DUT1\Semestre 2\M2204\Projet PILAF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7727022-8A87-4A4B-B3CB-953E998FF117}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FAEF59-BAE9-4590-9255-606C8D1BD57D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-9105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1233,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M76"/>
+  <dimension ref="A2:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1246,12 +1246,12 @@
     <col min="7" max="7" width="22.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -1259,12 +1259,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1304,12 +1304,8 @@
       <c r="G8" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="J8">
-        <f>IF(E8&gt;3,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1330,7 +1326,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1351,7 +1347,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1372,7 +1368,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +1389,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1414,7 +1410,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1435,7 +1431,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1456,7 +1452,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>22</v>
       </c>
@@ -1477,7 +1473,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
@@ -1498,7 +1494,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="25" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1540,7 +1536,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
@@ -1561,7 +1557,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1571,7 +1567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B22" s="12" t="s">
         <v>32</v>
       </c>
@@ -1583,12 +1579,12 @@
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
     </row>
-    <row r="25" spans="2:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="13" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="27" x14ac:dyDescent="0.3">
       <c r="B27" s="31" t="s">
         <v>35</v>
       </c>
@@ -1608,7 +1604,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>39</v>
       </c>
@@ -1628,12 +1624,8 @@
       <c r="G28" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="J28">
-        <f>IF(F28&gt;3,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>41</v>
       </c>
@@ -1653,18 +1645,8 @@
       <c r="G29" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J29">
-        <f t="shared" ref="J29:J35" si="2">IF(F29&gt;3,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>43</v>
       </c>
@@ -1684,18 +1666,8 @@
       <c r="G30" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>3</v>
-      </c>
-      <c r="M30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
@@ -1715,18 +1687,8 @@
       <c r="G31" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="J31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>5</v>
-      </c>
-      <c r="M31">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>46</v>
       </c>
@@ -1746,12 +1708,8 @@
       <c r="G32" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:8" ht="25" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>48</v>
       </c>
@@ -1771,12 +1729,8 @@
       <c r="G33" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="J33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>50</v>
       </c>
@@ -1796,12 +1750,8 @@
       <c r="G34" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="J34">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>52</v>
       </c>
@@ -1821,12 +1771,8 @@
       <c r="G35" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -1835,19 +1781,15 @@
         <f>SUM(F28:F35)</f>
         <v>5.5</v>
       </c>
-      <c r="J36">
-        <f>SUM(J28:J35)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="16"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
       <c r="F37" s="18"/>
     </row>
-    <row r="38" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="13" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
         <v>81</v>
       </c>
@@ -1859,22 +1801,22 @@
       <c r="E38" s="14"/>
       <c r="F38" s="15"/>
     </row>
-    <row r="41" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" ht="13" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="23" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="23" x14ac:dyDescent="0.25">
       <c r="B45" s="34" t="s">
         <v>58</v>
       </c>
@@ -1891,7 +1833,7 @@
       <c r="G45" s="35"/>
       <c r="H45" s="35"/>
     </row>
-    <row r="46" spans="2:10" ht="23" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="23" x14ac:dyDescent="0.25">
       <c r="B46" s="36" t="s">
         <v>59</v>
       </c>
@@ -1912,7 +1854,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="41" t="s">
         <v>63</v>
       </c>
@@ -1931,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="42"/>
       <c r="C48" s="39" t="s">
         <v>64</v>
@@ -2010,7 +1952,7 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4">
-        <f t="shared" ref="E55:E61" si="3">C55+D55</f>
+        <f t="shared" ref="E55:E61" si="2">C55+D55</f>
         <v>0</v>
       </c>
     </row>
@@ -2019,7 +1961,7 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2028,7 +1970,7 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2037,7 +1979,7 @@
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2046,7 +1988,7 @@
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2055,7 +1997,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2064,7 +2006,7 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2095,7 +2037,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="22"/>
     </row>
-    <row r="67" spans="2:6" ht="13" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="29" t="s">
         <v>80</v>
       </c>

</xml_diff>